<commit_message>
Remove MAIub from Pinus test
Changed name of obs data from Pinus.Stem.MAIub to MAIub, which should remove this variable from the test, which was providing a very low NSE value. Justified removal becuase only one site and narrow range of data
</commit_message>
<xml_diff>
--- a/Tests/Validation/Pinus/Observed.xlsx
+++ b/Tests/Validation/Pinus/Observed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Tests\UnderReview\Pinus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sme016\ApsimX\Tests\Validation\Pinus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6826AF87-3219-43A7-8249-20D3B75E97EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B063B816-35D8-4EFC-9261-8D00EC343A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17670" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="6" r:id="rId1"/>
@@ -303,9 +303,6 @@
     <t>Pinus.Stem.MAI</t>
   </si>
   <si>
-    <t>Pinus.Stem.MAIub</t>
-  </si>
-  <si>
     <t>LiveFoliarN</t>
   </si>
   <si>
@@ -397,6 +394,9 @@
   </si>
   <si>
     <t>FPQTuan_F2</t>
+  </si>
+  <si>
+    <t>MAIub</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1068,10 @@
   <dimension ref="A1:BT1505"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D1119" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1136" sqref="A1136"/>
+      <selection pane="bottomRight" activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -1124,13 +1124,13 @@
         <v>21</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F1" s="29" t="s">
         <v>56</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H1" s="29" t="s">
         <v>57</v>
@@ -1181,7 +1181,7 @@
         <v>34</v>
       </c>
       <c r="X1" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Y1" s="29" t="s">
         <v>2</v>
@@ -1211,34 +1211,34 @@
         <v>81</v>
       </c>
       <c r="AH1" s="44" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="AI1" s="29" t="s">
         <v>55</v>
       </c>
       <c r="AJ1" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AK1" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AL1" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM1" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="AM1" s="29" t="s">
+      <c r="AN1" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="AN1" s="29" t="s">
+      <c r="AO1" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="AO1" s="29" t="s">
-        <v>90</v>
-      </c>
       <c r="AP1" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ1" s="29" t="s">
         <v>83</v>
-      </c>
-      <c r="AQ1" s="29" t="s">
-        <v>84</v>
       </c>
       <c r="AR1" s="29" t="s">
         <v>10</v>
@@ -42573,7 +42573,7 @@
       <c r="AP1064" s="6"/>
       <c r="AQ1064" s="6"/>
       <c r="AR1064" s="35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AS1064" s="36"/>
       <c r="AT1064" s="36"/>
@@ -42647,7 +42647,7 @@
       <c r="AP1065" s="6"/>
       <c r="AQ1065" s="6"/>
       <c r="AR1065" s="35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AS1065" s="36"/>
       <c r="AT1065" s="36"/>
@@ -42721,7 +42721,7 @@
       <c r="AP1066" s="6"/>
       <c r="AQ1066" s="6"/>
       <c r="AR1066" s="35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AS1066" s="36"/>
       <c r="AT1066" s="36"/>
@@ -43658,7 +43658,7 @@
       <c r="AP1079" s="6"/>
       <c r="AQ1079" s="6"/>
       <c r="AR1079" s="35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AS1079" s="36"/>
       <c r="AT1079" s="36"/>
@@ -45849,7 +45849,7 @@
     </row>
     <row r="1136" spans="1:44">
       <c r="A1136" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1136" s="5">
         <v>35581.421999999999</v>
@@ -45870,7 +45870,7 @@
     </row>
     <row r="1137" spans="1:44">
       <c r="A1137" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1137" s="5">
         <v>35581.421999999999</v>
@@ -45891,7 +45891,7 @@
     </row>
     <row r="1138" spans="1:44">
       <c r="A1138" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1138" s="5">
         <v>35581.421999999999</v>
@@ -45912,7 +45912,7 @@
     </row>
     <row r="1139" spans="1:44">
       <c r="A1139" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1139" s="5">
         <v>35581.421999999999</v>
@@ -45933,7 +45933,7 @@
     </row>
     <row r="1140" spans="1:44">
       <c r="A1140" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1140" s="5">
         <v>35534.421999999999</v>
@@ -45954,7 +45954,7 @@
     </row>
     <row r="1141" spans="1:44">
       <c r="A1141" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1141" s="5">
         <v>35534.421999999999</v>
@@ -45975,7 +45975,7 @@
     </row>
     <row r="1142" spans="1:44">
       <c r="A1142" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B1142" s="5">
         <v>35534.421999999999</v>
@@ -45996,7 +45996,7 @@
     </row>
     <row r="1143" spans="1:44">
       <c r="A1143" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1143" s="5">
         <v>35534.421999999999</v>
@@ -46017,7 +46017,7 @@
     </row>
     <row r="1144" spans="1:44">
       <c r="A1144" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1144" s="5">
         <v>35550.421999999999</v>
@@ -46038,7 +46038,7 @@
     </row>
     <row r="1145" spans="1:44">
       <c r="A1145" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1145" s="5">
         <v>35550.421999999999</v>
@@ -46059,7 +46059,7 @@
     </row>
     <row r="1146" spans="1:44">
       <c r="A1146" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B1146" s="5">
         <v>35550.421999999999</v>
@@ -46080,7 +46080,7 @@
     </row>
     <row r="1147" spans="1:44">
       <c r="A1147" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1147" s="5">
         <v>35550.421999999999</v>
@@ -46101,7 +46101,7 @@
     </row>
     <row r="1148" spans="1:44">
       <c r="A1148" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1148" s="5">
         <v>37407.633000000002</v>
@@ -46133,7 +46133,7 @@
     </row>
     <row r="1149" spans="1:44">
       <c r="A1149" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1149" s="5">
         <v>37407.633000000002</v>
@@ -46165,7 +46165,7 @@
     </row>
     <row r="1150" spans="1:44">
       <c r="A1150" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1150" s="5">
         <v>37407.633000000002</v>
@@ -46197,7 +46197,7 @@
     </row>
     <row r="1151" spans="1:44">
       <c r="A1151" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1151" s="5">
         <v>37407.633000000002</v>
@@ -46229,7 +46229,7 @@
     </row>
     <row r="1152" spans="1:44">
       <c r="A1152" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1152" s="5">
         <v>37360.633000000002</v>
@@ -46261,7 +46261,7 @@
     </row>
     <row r="1153" spans="1:44">
       <c r="A1153" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1153" s="5">
         <v>37360.633000000002</v>
@@ -46293,7 +46293,7 @@
     </row>
     <row r="1154" spans="1:44">
       <c r="A1154" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B1154" s="5">
         <v>37360.633000000002</v>
@@ -46325,7 +46325,7 @@
     </row>
     <row r="1155" spans="1:44">
       <c r="A1155" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1155" s="5">
         <v>37360.633000000002</v>
@@ -46357,7 +46357,7 @@
     </row>
     <row r="1156" spans="1:44">
       <c r="A1156" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1156" s="5">
         <v>37376.633000000002</v>
@@ -46389,7 +46389,7 @@
     </row>
     <row r="1157" spans="1:44">
       <c r="A1157" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1157" s="5">
         <v>37376.633000000002</v>
@@ -46421,7 +46421,7 @@
     </row>
     <row r="1158" spans="1:44">
       <c r="A1158" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B1158" s="5">
         <v>37376.633000000002</v>
@@ -46453,7 +46453,7 @@
     </row>
     <row r="1159" spans="1:44">
       <c r="A1159" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1159" s="5">
         <v>37376.633000000002</v>
@@ -54480,7 +54480,7 @@
     </row>
     <row r="1439" spans="1:21" s="20" customFormat="1">
       <c r="A1439" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1439" s="5">
         <v>24303</v>
@@ -54499,7 +54499,7 @@
     </row>
     <row r="1440" spans="1:21" s="20" customFormat="1">
       <c r="A1440" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1440" s="5">
         <f>B$1439+365.25*C1440</f>
@@ -54520,7 +54520,7 @@
     </row>
     <row r="1441" spans="1:36" s="20" customFormat="1">
       <c r="A1441" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1441" s="5">
         <f>B$1439+365.25*C1441</f>
@@ -54571,7 +54571,7 @@
     </row>
     <row r="1442" spans="1:36">
       <c r="A1442" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1442" s="5">
         <v>35200</v>
@@ -54594,7 +54594,7 @@
     </row>
     <row r="1443" spans="1:36">
       <c r="A1443" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1443" s="5">
         <f>B$1442+365.25*C1443</f>
@@ -54618,7 +54618,7 @@
     </row>
     <row r="1444" spans="1:36">
       <c r="A1444" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1444" s="5">
         <f t="shared" ref="B1444:B1449" si="18">B$1442+365.25*C1444</f>
@@ -54647,7 +54647,7 @@
     </row>
     <row r="1445" spans="1:36">
       <c r="A1445" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1445" s="5">
         <f t="shared" ref="B1445" si="19">B$1442+365.25*C1445</f>
@@ -54693,7 +54693,7 @@
     </row>
     <row r="1446" spans="1:36">
       <c r="A1446" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1446" s="5">
         <f t="shared" si="18"/>
@@ -54747,7 +54747,7 @@
     </row>
     <row r="1447" spans="1:36">
       <c r="A1447" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1447" s="5">
         <f t="shared" si="18"/>
@@ -54778,7 +54778,7 @@
     </row>
     <row r="1448" spans="1:36">
       <c r="A1448" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1448" s="5">
         <f t="shared" si="18"/>
@@ -54809,7 +54809,7 @@
     </row>
     <row r="1449" spans="1:36">
       <c r="A1449" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1449" s="5">
         <f t="shared" si="18"/>
@@ -54842,7 +54842,7 @@
     </row>
     <row r="1450" spans="1:36">
       <c r="A1450" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1450" s="54">
         <v>36600</v>
@@ -54859,7 +54859,7 @@
     </row>
     <row r="1451" spans="1:36">
       <c r="A1451" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1451" s="5">
         <f>B$1450+365.25*C1451</f>
@@ -54890,7 +54890,7 @@
     </row>
     <row r="1452" spans="1:36">
       <c r="A1452" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1452" s="5">
         <f t="shared" ref="B1452:B1455" si="20">B$1450+365.25*C1452</f>
@@ -54921,7 +54921,7 @@
     </row>
     <row r="1453" spans="1:36">
       <c r="A1453" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1453" s="5">
         <f t="shared" si="20"/>
@@ -54954,7 +54954,7 @@
     </row>
     <row r="1454" spans="1:36">
       <c r="A1454" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1454" s="5">
         <f t="shared" si="20"/>
@@ -54975,7 +54975,7 @@
     </row>
     <row r="1455" spans="1:36">
       <c r="A1455" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1455" s="5">
         <f t="shared" si="20"/>
@@ -55001,7 +55001,7 @@
     </row>
     <row r="1456" spans="1:36">
       <c r="A1456" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1456" s="54">
         <v>37408</v>
@@ -55018,7 +55018,7 @@
     </row>
     <row r="1457" spans="1:32">
       <c r="A1457" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1457" s="54">
         <f>B$1456+365.25*C1457</f>
@@ -55043,7 +55043,7 @@
     </row>
     <row r="1458" spans="1:32">
       <c r="A1458" s="56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1458" s="5">
         <v>36285</v>
@@ -55060,7 +55060,7 @@
     </row>
     <row r="1459" spans="1:32">
       <c r="A1459" s="56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1459" s="54">
         <f>B$1458+365.25*C1459</f>
@@ -55083,7 +55083,7 @@
     </row>
     <row r="1460" spans="1:32">
       <c r="A1460" s="56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1460" s="54">
         <f t="shared" ref="B1460" si="21">B$1458+365.25*C1460</f>
@@ -55115,7 +55115,7 @@
     </row>
     <row r="1461" spans="1:32">
       <c r="A1461" s="56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1461" s="54">
         <f>B$1458+365.25*C1461</f>
@@ -55147,7 +55147,7 @@
     </row>
     <row r="1462" spans="1:32">
       <c r="A1462" s="56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1462" s="54">
         <f>B$1458+365.25*C1462</f>
@@ -55167,7 +55167,7 @@
     </row>
     <row r="1463" spans="1:32">
       <c r="A1463" s="56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1463" s="54">
         <f>B$1458+365.25*C1463</f>
@@ -55199,7 +55199,7 @@
     </row>
     <row r="1464" spans="1:32">
       <c r="A1464" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1464" s="54">
         <v>13346</v>
@@ -55216,7 +55216,7 @@
     </row>
     <row r="1465" spans="1:32">
       <c r="A1465" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1465" s="54">
         <f>B$1464+365.25*C1465</f>
@@ -55241,7 +55241,7 @@
     </row>
     <row r="1466" spans="1:32">
       <c r="A1466" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1466" s="54">
         <f t="shared" ref="B1466:B1481" si="23">B$1464+365.25*C1466</f>
@@ -55266,7 +55266,7 @@
     </row>
     <row r="1467" spans="1:32">
       <c r="A1467" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1467" s="54">
         <f t="shared" si="23"/>
@@ -55291,7 +55291,7 @@
     </row>
     <row r="1468" spans="1:32">
       <c r="A1468" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1468" s="54">
         <f t="shared" si="23"/>
@@ -55316,7 +55316,7 @@
     </row>
     <row r="1469" spans="1:32">
       <c r="A1469" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1469" s="54">
         <f t="shared" si="23"/>
@@ -55341,7 +55341,7 @@
     </row>
     <row r="1470" spans="1:32">
       <c r="A1470" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1470" s="54">
         <f t="shared" si="23"/>
@@ -55366,7 +55366,7 @@
     </row>
     <row r="1471" spans="1:32">
       <c r="A1471" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1471" s="54">
         <f t="shared" si="23"/>
@@ -55389,7 +55389,7 @@
     </row>
     <row r="1472" spans="1:32">
       <c r="A1472" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1472" s="54">
         <f t="shared" si="23"/>
@@ -55414,7 +55414,7 @@
     </row>
     <row r="1473" spans="1:30">
       <c r="A1473" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1473" s="54">
         <f t="shared" si="23"/>
@@ -55437,7 +55437,7 @@
     </row>
     <row r="1474" spans="1:30">
       <c r="A1474" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1474" s="54">
         <f t="shared" si="23"/>
@@ -55460,7 +55460,7 @@
     </row>
     <row r="1475" spans="1:30">
       <c r="A1475" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1475" s="54">
         <f t="shared" si="23"/>
@@ -55485,7 +55485,7 @@
     </row>
     <row r="1476" spans="1:30">
       <c r="A1476" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1476" s="54">
         <f t="shared" si="23"/>
@@ -55508,7 +55508,7 @@
     </row>
     <row r="1477" spans="1:30">
       <c r="A1477" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1477" s="54">
         <f t="shared" si="23"/>
@@ -55533,7 +55533,7 @@
     </row>
     <row r="1478" spans="1:30">
       <c r="A1478" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1478" s="54">
         <f t="shared" si="23"/>
@@ -55556,7 +55556,7 @@
     </row>
     <row r="1479" spans="1:30">
       <c r="A1479" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1479" s="54">
         <f t="shared" si="23"/>
@@ -55579,7 +55579,7 @@
     </row>
     <row r="1480" spans="1:30">
       <c r="A1480" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1480" s="54">
         <f t="shared" si="23"/>
@@ -55604,7 +55604,7 @@
     </row>
     <row r="1481" spans="1:30">
       <c r="A1481" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1481" s="54">
         <f t="shared" si="23"/>
@@ -55622,7 +55622,7 @@
     </row>
     <row r="1482" spans="1:30">
       <c r="A1482" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1482" s="54">
         <f>B$1481+365.25*C1482</f>
@@ -55647,7 +55647,7 @@
     </row>
     <row r="1483" spans="1:30">
       <c r="A1483" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1483" s="54">
         <f t="shared" ref="B1483:B1505" si="25">B$1481+365.25*C1483</f>
@@ -55672,7 +55672,7 @@
     </row>
     <row r="1484" spans="1:30">
       <c r="A1484" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1484" s="54">
         <f t="shared" si="25"/>
@@ -55697,7 +55697,7 @@
     </row>
     <row r="1485" spans="1:30">
       <c r="A1485" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1485" s="54">
         <f t="shared" si="25"/>
@@ -55722,7 +55722,7 @@
     </row>
     <row r="1486" spans="1:30">
       <c r="A1486" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1486" s="54">
         <f t="shared" si="25"/>
@@ -55747,7 +55747,7 @@
     </row>
     <row r="1487" spans="1:30">
       <c r="A1487" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1487" s="54">
         <f t="shared" si="25"/>
@@ -55770,7 +55770,7 @@
     </row>
     <row r="1488" spans="1:30">
       <c r="A1488" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1488" s="54">
         <f t="shared" si="25"/>
@@ -55795,7 +55795,7 @@
     </row>
     <row r="1489" spans="1:30">
       <c r="A1489" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1489" s="54">
         <f t="shared" si="25"/>
@@ -55818,7 +55818,7 @@
     </row>
     <row r="1490" spans="1:30">
       <c r="A1490" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1490" s="54">
         <f t="shared" si="25"/>
@@ -55841,7 +55841,7 @@
     </row>
     <row r="1491" spans="1:30">
       <c r="A1491" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1491" s="54">
         <f t="shared" si="25"/>
@@ -55866,7 +55866,7 @@
     </row>
     <row r="1492" spans="1:30">
       <c r="A1492" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1492" s="54">
         <f t="shared" si="25"/>
@@ -55889,7 +55889,7 @@
     </row>
     <row r="1493" spans="1:30">
       <c r="A1493" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1493" s="54">
         <f t="shared" si="25"/>
@@ -55912,7 +55912,7 @@
     </row>
     <row r="1494" spans="1:30">
       <c r="A1494" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1494" s="54">
         <f t="shared" si="25"/>
@@ -55937,7 +55937,7 @@
     </row>
     <row r="1495" spans="1:30">
       <c r="A1495" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1495" s="54">
         <f t="shared" si="25"/>
@@ -55962,7 +55962,7 @@
     </row>
     <row r="1496" spans="1:30">
       <c r="A1496" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1496" s="54">
         <f t="shared" si="25"/>
@@ -55987,7 +55987,7 @@
     </row>
     <row r="1497" spans="1:30">
       <c r="A1497" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1497" s="54">
         <f t="shared" si="25"/>
@@ -56010,7 +56010,7 @@
     </row>
     <row r="1498" spans="1:30">
       <c r="A1498" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1498" s="54">
         <f t="shared" si="25"/>
@@ -56035,7 +56035,7 @@
     </row>
     <row r="1499" spans="1:30">
       <c r="A1499" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1499" s="54">
         <f t="shared" si="25"/>
@@ -56060,7 +56060,7 @@
     </row>
     <row r="1500" spans="1:30">
       <c r="A1500" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1500" s="54">
         <f t="shared" si="25"/>
@@ -56083,7 +56083,7 @@
     </row>
     <row r="1501" spans="1:30">
       <c r="A1501" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1501" s="54">
         <f t="shared" si="25"/>
@@ -56106,7 +56106,7 @@
     </row>
     <row r="1502" spans="1:30">
       <c r="A1502" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1502" s="54">
         <f t="shared" si="25"/>
@@ -56129,7 +56129,7 @@
     </row>
     <row r="1503" spans="1:30">
       <c r="A1503" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1503" s="54">
         <f t="shared" si="25"/>
@@ -56154,7 +56154,7 @@
     </row>
     <row r="1504" spans="1:30">
       <c r="A1504" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1504" s="54">
         <f t="shared" si="25"/>
@@ -56177,7 +56177,7 @@
     </row>
     <row r="1505" spans="1:30">
       <c r="A1505" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1505" s="54">
         <f t="shared" si="25"/>

</xml_diff>